<commit_message>
updated generation limit keys
</commit_message>
<xml_diff>
--- a/source_files/RE Capacity for Model.xlsx
+++ b/source_files/RE Capacity for Model.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" tabRatio="548"/>
   </bookViews>
   <sheets>
-    <sheet name="RE Capacity For Model" sheetId="9" r:id="rId1"/>
-    <sheet name="RE Capacity by project" sheetId="8" r:id="rId2"/>
+    <sheet name="RE Capacity by project" sheetId="8" r:id="rId1"/>
+    <sheet name="RE Capacity For Model" sheetId="9" r:id="rId2"/>
     <sheet name="Hydro Capacity for model" sheetId="6" r:id="rId3"/>
     <sheet name="Wind Capacity For Model" sheetId="7" r:id="rId4"/>
     <sheet name="Data" sheetId="1" r:id="rId5"/>
@@ -29,7 +29,7 @@
   <calcPr calcId="162913"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="4" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="343">
   <si>
     <t>Service Area</t>
   </si>
@@ -1130,6 +1130,27 @@
   </si>
   <si>
     <t>Sum of Average Annual Generation (kWh)</t>
+  </si>
+  <si>
+    <t>Ketchikan_intertie</t>
+  </si>
+  <si>
+    <t>Craig_intertie</t>
+  </si>
+  <si>
+    <t>Kodiak_intertie</t>
+  </si>
+  <si>
+    <t>Haines_intertie</t>
+  </si>
+  <si>
+    <t>Valdez</t>
+  </si>
+  <si>
+    <t>Newhalen_intertie</t>
+  </si>
+  <si>
+    <t>Toksook_Bay_intertie</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1159,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1386,16 +1407,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -2239,7 +2260,7 @@
     <cacheField name="Capacity (kW)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="120000"/>
     </cacheField>
-    <cacheField name="Average Annual Generation (kWh)" numFmtId="166">
+    <cacheField name="Average Annual Generation (kWh)" numFmtId="164">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="380000000"/>
     </cacheField>
   </cacheFields>
@@ -4896,7 +4917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D52" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
@@ -6099,9 +6120,1481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="37"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>105</v>
+      </c>
+      <c r="F2" s="41">
+        <v>312652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>284</v>
+      </c>
+      <c r="F3" s="41">
+        <v>443142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4" s="41">
+        <v>1103760</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5" s="41">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>167</v>
+      </c>
+      <c r="F6" s="41">
+        <v>521200.00000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>1250</v>
+      </c>
+      <c r="F7" s="41">
+        <v>3553542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>6000</v>
+      </c>
+      <c r="F8" s="41">
+        <v>15929397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E9">
+        <v>400</v>
+      </c>
+      <c r="F9" s="41">
+        <v>699206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E10">
+        <v>300</v>
+      </c>
+      <c r="F10" s="41">
+        <v>1103760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>340</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>6500</v>
+      </c>
+      <c r="F11" s="41">
+        <v>15056617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>12000</v>
+      </c>
+      <c r="F12" s="41">
+        <v>45000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>800</v>
+      </c>
+      <c r="F13" s="41">
+        <v>1939011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>600</v>
+      </c>
+      <c r="F14" s="41">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>943</v>
+      </c>
+      <c r="F15" s="41">
+        <v>3137760</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>4000</v>
+      </c>
+      <c r="F16" s="41">
+        <v>15617000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>339</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>3000</v>
+      </c>
+      <c r="F17" s="41">
+        <v>7446440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>285</v>
+      </c>
+      <c r="F18" s="41">
+        <v>164432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>450</v>
+      </c>
+      <c r="F19" s="41">
+        <v>1810000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>307</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E20">
+        <v>300</v>
+      </c>
+      <c r="F20" s="41">
+        <v>814680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>341</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>824</v>
+      </c>
+      <c r="F21" s="41">
+        <v>4048161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>4000</v>
+      </c>
+      <c r="F22" s="41">
+        <v>26000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>1600</v>
+      </c>
+      <c r="F23" s="41">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>14300</v>
+      </c>
+      <c r="F24" s="41">
+        <v>75000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25">
+        <v>8500</v>
+      </c>
+      <c r="F25" s="41">
+        <v>29500000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26">
+        <v>78200</v>
+      </c>
+      <c r="F26" s="41">
+        <v>295000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>303</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E27">
+        <v>300</v>
+      </c>
+      <c r="F27" s="41">
+        <v>840960</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>800</v>
+      </c>
+      <c r="F28" s="41">
+        <v>1997981</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>338</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>34000</v>
+      </c>
+      <c r="F29" s="41">
+        <v>135000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>338</v>
+      </c>
+      <c r="B30" t="s">
+        <v>331</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E30">
+        <v>9000</v>
+      </c>
+      <c r="F30" s="41">
+        <v>26017200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>317</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E31">
+        <v>180</v>
+      </c>
+      <c r="F31" s="41">
+        <v>531381.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>316</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E32">
+        <v>475</v>
+      </c>
+      <c r="F32" s="41">
+        <v>1019445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>298</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E33">
+        <v>1800</v>
+      </c>
+      <c r="F33" s="41">
+        <v>4478112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E34">
+        <v>475</v>
+      </c>
+      <c r="F34" s="41">
+        <v>4173184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>475</v>
+      </c>
+      <c r="F35" s="41">
+        <v>773021</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>313</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E36">
+        <v>200</v>
+      </c>
+      <c r="F36" s="41">
+        <v>480048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>1100</v>
+      </c>
+      <c r="F37" s="41">
+        <v>4960915</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>3900</v>
+      </c>
+      <c r="F38" s="41">
+        <v>16075775</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>314</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E39">
+        <v>65</v>
+      </c>
+      <c r="F39" s="41">
+        <v>204984</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>328</v>
+      </c>
+      <c r="B40" t="s">
+        <v>330</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E40">
+        <v>2970</v>
+      </c>
+      <c r="F40" s="41">
+        <v>5960707</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>125</v>
+      </c>
+      <c r="F41" s="41">
+        <v>167000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42">
+        <v>650</v>
+      </c>
+      <c r="F42" s="41">
+        <v>799494</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>308</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E43">
+        <v>24</v>
+      </c>
+      <c r="F43" s="41">
+        <v>31536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>254</v>
+      </c>
+      <c r="B44" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D44" t="s">
+        <v>277</v>
+      </c>
+      <c r="E44">
+        <v>249</v>
+      </c>
+      <c r="F44" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>266</v>
+      </c>
+      <c r="B45" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D45" t="s">
+        <v>277</v>
+      </c>
+      <c r="E45">
+        <v>75</v>
+      </c>
+      <c r="F45" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>337</v>
+      </c>
+      <c r="B46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46">
+        <v>4500</v>
+      </c>
+      <c r="F46" s="41">
+        <v>20600350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>337</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47">
+        <v>2000</v>
+      </c>
+      <c r="F47" s="41">
+        <v>5739704</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>337</v>
+      </c>
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48">
+        <v>4775</v>
+      </c>
+      <c r="F48" s="41">
+        <v>25250000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>312</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E49">
+        <v>300</v>
+      </c>
+      <c r="F49" s="41">
+        <v>620208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50">
+        <v>750</v>
+      </c>
+      <c r="F50" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51">
+        <v>120000</v>
+      </c>
+      <c r="F51" s="41">
+        <v>380000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D52" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="41">
+        <v>6020000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53">
+        <v>19200</v>
+      </c>
+      <c r="F53" s="41">
+        <v>42000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54">
+        <v>40000</v>
+      </c>
+      <c r="F54" s="41">
+        <v>172076600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>189</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>160</v>
+      </c>
+      <c r="F55" s="41">
+        <v>876000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56">
+        <v>125</v>
+      </c>
+      <c r="F56" s="41">
+        <v>386567</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>1200</v>
+      </c>
+      <c r="F57" s="41">
+        <v>3724910</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>305</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E58">
+        <v>1000</v>
+      </c>
+      <c r="F58" s="41">
+        <v>2076120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>321</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E59">
+        <v>24600</v>
+      </c>
+      <c r="F59" s="41">
+        <v>73268640</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>320</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E60">
+        <v>17600</v>
+      </c>
+      <c r="F60" s="41">
+        <v>47794560</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>302</v>
+      </c>
+      <c r="B61" t="s">
+        <v>333</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E61">
+        <v>225</v>
+      </c>
+      <c r="F61" s="41">
+        <v>696748.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>315</v>
+      </c>
+      <c r="B62" t="s">
+        <v>332</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E62">
+        <v>1000</v>
+      </c>
+      <c r="F62" s="41">
+        <v>1408608</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>306</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E63">
+        <v>200</v>
+      </c>
+      <c r="F63" s="41">
+        <v>579912</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>300</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E64">
+        <v>260</v>
+      </c>
+      <c r="F64" s="41">
+        <v>296088</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>319</v>
+      </c>
+      <c r="C65" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E65">
+        <v>200</v>
+      </c>
+      <c r="F65" s="41">
+        <v>411720</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66">
+        <v>15645</v>
+      </c>
+      <c r="F66" s="41">
+        <v>100200000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67">
+        <v>18600</v>
+      </c>
+      <c r="F67" s="41">
+        <v>63800000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>180</v>
+      </c>
+      <c r="F68" s="41">
+        <v>1169000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>304</v>
+      </c>
+      <c r="C69" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E69">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>342</v>
+      </c>
+      <c r="C70" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E70">
+        <v>400</v>
+      </c>
+      <c r="F70" s="41">
+        <v>219000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>323</v>
+      </c>
+      <c r="C71" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E71">
+        <v>475</v>
+      </c>
+      <c r="F71" s="41">
+        <v>865488</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>309</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E72">
+        <v>600</v>
+      </c>
+      <c r="F72" s="41">
+        <v>1093248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>299</v>
+      </c>
+      <c r="C73" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="E73">
+        <v>130</v>
+      </c>
+      <c r="F73" s="41">
+        <v>398580</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>336</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D74" t="s">
+        <v>119</v>
+      </c>
+      <c r="E74">
+        <v>5200</v>
+      </c>
+      <c r="F74" s="41">
+        <v>44675500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>336</v>
+      </c>
+      <c r="B75" t="s">
+        <v>240</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" t="s">
+        <v>17</v>
+      </c>
+      <c r="E75">
+        <v>2000</v>
+      </c>
+      <c r="F75" s="41">
+        <v>982000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76">
+        <v>4200</v>
+      </c>
+      <c r="F76" s="41">
+        <v>23025300</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>336</v>
+      </c>
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77">
+        <v>2100</v>
+      </c>
+      <c r="F77" s="41">
+        <v>12461600</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>336</v>
+      </c>
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+      <c r="C78" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D78" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78">
+        <v>22500</v>
+      </c>
+      <c r="F78" s="41">
+        <v>76000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>336</v>
+      </c>
+      <c r="B79" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79">
+        <v>22500</v>
+      </c>
+      <c r="F79" s="41">
+        <v>125000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>336</v>
+      </c>
+      <c r="B80" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="D80" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80">
+        <v>4600</v>
+      </c>
+      <c r="F80" s="41">
+        <v>16000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F80">
+    <sortCondition ref="A2:A80"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
@@ -6837,1478 +8330,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F80"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F80"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="37"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="41" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>334</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>292</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>105</v>
-      </c>
-      <c r="F2" s="41">
-        <v>312652</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>284</v>
-      </c>
-      <c r="F3" s="41">
-        <v>443142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E4">
-        <v>400</v>
-      </c>
-      <c r="F4" s="41">
-        <v>1103760</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-      <c r="F5" s="41">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>167</v>
-      </c>
-      <c r="F6" s="41">
-        <v>521200.00000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>1250</v>
-      </c>
-      <c r="F7" s="41">
-        <v>3553542</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>6000</v>
-      </c>
-      <c r="F8" s="41">
-        <v>15929397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E9">
-        <v>400</v>
-      </c>
-      <c r="F9" s="41">
-        <v>699206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E10">
-        <v>300</v>
-      </c>
-      <c r="F10" s="41">
-        <v>1103760</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>6500</v>
-      </c>
-      <c r="F11" s="41">
-        <v>15056617</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <v>12000</v>
-      </c>
-      <c r="F12" s="41">
-        <v>45000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>800</v>
-      </c>
-      <c r="F13" s="41">
-        <v>1939011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>600</v>
-      </c>
-      <c r="F14" s="41">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>943</v>
-      </c>
-      <c r="F15" s="41">
-        <v>3137760</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16">
-        <v>4000</v>
-      </c>
-      <c r="F16" s="41">
-        <v>15617000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <v>3000</v>
-      </c>
-      <c r="F17" s="41">
-        <v>7446440</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>285</v>
-      </c>
-      <c r="F18" s="41">
-        <v>164432</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19">
-        <v>450</v>
-      </c>
-      <c r="F19" s="41">
-        <v>1810000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>307</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E20">
-        <v>300</v>
-      </c>
-      <c r="F20" s="41">
-        <v>814680</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21">
-        <v>824</v>
-      </c>
-      <c r="F21" s="41">
-        <v>4048161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22">
-        <v>4000</v>
-      </c>
-      <c r="F22" s="41">
-        <v>26000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23">
-        <v>1600</v>
-      </c>
-      <c r="F23" s="41">
-        <v>4500000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>14300</v>
-      </c>
-      <c r="F24" s="41">
-        <v>75000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25">
-        <v>8500</v>
-      </c>
-      <c r="F25" s="41">
-        <v>29500000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26">
-        <v>78200</v>
-      </c>
-      <c r="F26" s="41">
-        <v>295000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>303</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E27">
-        <v>300</v>
-      </c>
-      <c r="F27" s="41">
-        <v>840960</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28">
-        <v>800</v>
-      </c>
-      <c r="F28" s="41">
-        <v>1997981</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29">
-        <v>34000</v>
-      </c>
-      <c r="F29" s="41">
-        <v>135000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" t="s">
-        <v>331</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E30">
-        <v>9000</v>
-      </c>
-      <c r="F30" s="41">
-        <v>26017200</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>317</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E31">
-        <v>180</v>
-      </c>
-      <c r="F31" s="41">
-        <v>531381.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>316</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E32">
-        <v>475</v>
-      </c>
-      <c r="F32" s="41">
-        <v>1019445</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C33" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E33">
-        <v>1800</v>
-      </c>
-      <c r="F33" s="41">
-        <v>4478112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>322</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E34">
-        <v>475</v>
-      </c>
-      <c r="F34" s="41">
-        <v>4173184</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35">
-        <v>475</v>
-      </c>
-      <c r="F35" s="41">
-        <v>773021</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>313</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E36">
-        <v>200</v>
-      </c>
-      <c r="F36" s="41">
-        <v>480048</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37">
-        <v>1100</v>
-      </c>
-      <c r="F37" s="41">
-        <v>4960915</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <v>3900</v>
-      </c>
-      <c r="F38" s="41">
-        <v>16075775</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>314</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E39">
-        <v>65</v>
-      </c>
-      <c r="F39" s="41">
-        <v>204984</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>328</v>
-      </c>
-      <c r="B40" t="s">
-        <v>330</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E40">
-        <v>2970</v>
-      </c>
-      <c r="F40" s="41">
-        <v>5960707</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41">
-        <v>125</v>
-      </c>
-      <c r="F41" s="41">
-        <v>167000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42">
-        <v>650</v>
-      </c>
-      <c r="F42" s="41">
-        <v>799494</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>308</v>
-      </c>
-      <c r="C43" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E43">
-        <v>24</v>
-      </c>
-      <c r="F43" s="41">
-        <v>31536</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>254</v>
-      </c>
-      <c r="B44" t="s">
-        <v>252</v>
-      </c>
-      <c r="C44" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D44" t="s">
-        <v>277</v>
-      </c>
-      <c r="E44">
-        <v>249</v>
-      </c>
-      <c r="F44" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>266</v>
-      </c>
-      <c r="B45" t="s">
-        <v>255</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D45" t="s">
-        <v>277</v>
-      </c>
-      <c r="E45">
-        <v>75</v>
-      </c>
-      <c r="F45" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46">
-        <v>4500</v>
-      </c>
-      <c r="F46" s="41">
-        <v>20600350</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47">
-        <v>2000</v>
-      </c>
-      <c r="F47" s="41">
-        <v>5739704</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" t="s">
-        <v>148</v>
-      </c>
-      <c r="C48" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D48" t="s">
-        <v>17</v>
-      </c>
-      <c r="E48">
-        <v>4775</v>
-      </c>
-      <c r="F48" s="41">
-        <v>25250000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>312</v>
-      </c>
-      <c r="C49" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E49">
-        <v>300</v>
-      </c>
-      <c r="F49" s="41">
-        <v>620208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D50" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50">
-        <v>750</v>
-      </c>
-      <c r="F50" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D51" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51">
-        <v>120000</v>
-      </c>
-      <c r="F51" s="41">
-        <v>380000000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>60</v>
-      </c>
-      <c r="B52" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D52" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52" s="41">
-        <v>6020000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53">
-        <v>19200</v>
-      </c>
-      <c r="F53" s="41">
-        <v>42000000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D54" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54">
-        <v>40000</v>
-      </c>
-      <c r="F54" s="41">
-        <v>172076600</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" t="s">
-        <v>189</v>
-      </c>
-      <c r="C55" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55">
-        <v>160</v>
-      </c>
-      <c r="F55" s="41">
-        <v>876000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56">
-        <v>125</v>
-      </c>
-      <c r="F56" s="41">
-        <v>386567</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" t="s">
-        <v>59</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57">
-        <v>1200</v>
-      </c>
-      <c r="F57" s="41">
-        <v>3724910</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" t="s">
-        <v>305</v>
-      </c>
-      <c r="C58" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E58">
-        <v>1000</v>
-      </c>
-      <c r="F58" s="41">
-        <v>2076120</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" t="s">
-        <v>321</v>
-      </c>
-      <c r="C59" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E59">
-        <v>24600</v>
-      </c>
-      <c r="F59" s="41">
-        <v>73268640</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" t="s">
-        <v>320</v>
-      </c>
-      <c r="C60" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E60">
-        <v>17600</v>
-      </c>
-      <c r="F60" s="41">
-        <v>47794560</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>302</v>
-      </c>
-      <c r="B61" t="s">
-        <v>333</v>
-      </c>
-      <c r="C61" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E61">
-        <v>225</v>
-      </c>
-      <c r="F61" s="41">
-        <v>696748.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>315</v>
-      </c>
-      <c r="B62" t="s">
-        <v>332</v>
-      </c>
-      <c r="C62" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E62">
-        <v>1000</v>
-      </c>
-      <c r="F62" s="41">
-        <v>1408608</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>306</v>
-      </c>
-      <c r="C63" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E63">
-        <v>200</v>
-      </c>
-      <c r="F63" s="41">
-        <v>579912</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>300</v>
-      </c>
-      <c r="C64" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E64">
-        <v>260</v>
-      </c>
-      <c r="F64" s="41">
-        <v>296088</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>319</v>
-      </c>
-      <c r="C65" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E65">
-        <v>200</v>
-      </c>
-      <c r="F65" s="41">
-        <v>411720</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" t="s">
-        <v>199</v>
-      </c>
-      <c r="C66" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D66" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66">
-        <v>15645</v>
-      </c>
-      <c r="F66" s="41">
-        <v>100200000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D67" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67">
-        <v>18600</v>
-      </c>
-      <c r="F67" s="41">
-        <v>63800000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" t="s">
-        <v>79</v>
-      </c>
-      <c r="C68" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68">
-        <v>180</v>
-      </c>
-      <c r="F68" s="41">
-        <v>1169000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>304</v>
-      </c>
-      <c r="C69" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E69">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>301</v>
-      </c>
-      <c r="C70" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E70">
-        <v>400</v>
-      </c>
-      <c r="F70" s="41">
-        <v>219000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>323</v>
-      </c>
-      <c r="C71" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E71">
-        <v>475</v>
-      </c>
-      <c r="F71" s="41">
-        <v>865488</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>309</v>
-      </c>
-      <c r="C72" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E72">
-        <v>600</v>
-      </c>
-      <c r="F72" s="41">
-        <v>1093248</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>299</v>
-      </c>
-      <c r="C73" s="37" t="s">
-        <v>326</v>
-      </c>
-      <c r="E73">
-        <v>130</v>
-      </c>
-      <c r="F73" s="41">
-        <v>398580</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>278</v>
-      </c>
-      <c r="B74" t="s">
-        <v>53</v>
-      </c>
-      <c r="C74" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D74" t="s">
-        <v>119</v>
-      </c>
-      <c r="E74">
-        <v>5200</v>
-      </c>
-      <c r="F74" s="41">
-        <v>44675500</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>278</v>
-      </c>
-      <c r="B75" t="s">
-        <v>240</v>
-      </c>
-      <c r="C75" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D75" t="s">
-        <v>17</v>
-      </c>
-      <c r="E75">
-        <v>2000</v>
-      </c>
-      <c r="F75" s="41">
-        <v>982000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>278</v>
-      </c>
-      <c r="B76" t="s">
-        <v>55</v>
-      </c>
-      <c r="C76" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D76" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76">
-        <v>4200</v>
-      </c>
-      <c r="F76" s="41">
-        <v>23025300</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B77" t="s">
-        <v>56</v>
-      </c>
-      <c r="C77" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D77" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77">
-        <v>2100</v>
-      </c>
-      <c r="F77" s="41">
-        <v>12461600</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>278</v>
-      </c>
-      <c r="B78" t="s">
-        <v>70</v>
-      </c>
-      <c r="C78" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D78" t="s">
-        <v>17</v>
-      </c>
-      <c r="E78">
-        <v>22500</v>
-      </c>
-      <c r="F78" s="41">
-        <v>76000000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>278</v>
-      </c>
-      <c r="B79" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D79" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79">
-        <v>22500</v>
-      </c>
-      <c r="F79" s="41">
-        <v>125000000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>278</v>
-      </c>
-      <c r="B80" t="s">
-        <v>57</v>
-      </c>
-      <c r="C80" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="D80" t="s">
-        <v>17</v>
-      </c>
-      <c r="E80">
-        <v>4600</v>
-      </c>
-      <c r="F80" s="41">
-        <v>16000000</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:F80">
-    <sortCondition ref="A2:A80"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>